<commit_message>
using id's in kuvio specification yamls
</commit_message>
<xml_diff>
--- a/ptt_ennusteet_KT_uusi_sarja_id.xlsx
+++ b/ptt_ennusteet_KT_uusi_sarja_id.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">muunnos</t>
   </si>
   <si>
-    <t xml:space="preserve">data('StatFin/kan/ntp/statfin_ntp_pxt_132h.px', tidy_time=TRUE)|&gt;filter(Taloustoimi=='B1GMH Bruttokansantuote markkinahintaan')|&gt;filter(Tiedot=='Kausitasoitettu ja työpäiväkorjattu sarja, viitevuosi 2015, miljoonaa euroa')</t>
+    <t xml:space="preserve">bkt_ennuste</t>
   </si>
   <si>
     <t xml:space="preserve">BKT</t>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">vuosimuutos</t>
   </si>
   <si>
-    <t xml:space="preserve">data('StatFin/kan/ntp/statfin_ntp_pxt_132h.px', tidy_time=TRUE)|&gt;filter(Taloustoimi=='P3KS14_S15 Yksityiset kulutusmenot, menona')|&gt;filter(Tiedot=='Kausitasoitettu ja työpäiväkorjattu sarja, viitevuosi 2015, miljoonaa euroa')</t>
+    <t xml:space="preserve">yksityinen_kulutus_ennuste</t>
   </si>
   <si>
     <t xml:space="preserve">Yksityinen kulutus</t>
@@ -265,7 +265,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>